<commit_message>
Agregado Logo y Factura
</commit_message>
<xml_diff>
--- a/DiccionarioDatos.xlsx
+++ b/DiccionarioDatos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianSegura\source\repos\JulianSegura\DreamSky_RentShop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CEF158-EBDB-4499-9122-383ED389A05D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459C0DAF-17E3-4BD6-9D4C-DFFF84350B3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{2B2B9735-A783-4B16-AC2F-26E56F42E022}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="73">
   <si>
     <t>Campo</t>
   </si>
@@ -234,9 +234,6 @@
     <t>GetDate Automatico</t>
   </si>
   <si>
-    <t>TiposRNC</t>
-  </si>
-  <si>
     <t>IdFactura</t>
   </si>
   <si>
@@ -247,6 +244,12 @@
   </si>
   <si>
     <t>Descuento</t>
+  </si>
+  <si>
+    <t>TiposNCF</t>
+  </si>
+  <si>
+    <t>Estado</t>
   </si>
 </sst>
 </file>
@@ -322,12 +325,6 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -336,6 +333,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -653,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC292F6-2220-4649-8829-258F1E686873}">
   <dimension ref="A1:U70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,33 +675,37 @@
     <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="F1" s="1" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="K1" s="1" t="s">
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="K1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="R1" s="1" t="s">
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="R1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -707,7 +714,7 @@
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
@@ -719,7 +726,7 @@
       <c r="G2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I2" t="s">
@@ -731,7 +738,7 @@
       <c r="L2" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="N2" t="s">
@@ -743,7 +750,7 @@
       <c r="S2" t="s">
         <v>1</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="U2" t="s">
@@ -757,7 +764,7 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
@@ -769,7 +776,7 @@
       <c r="G3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I3" t="s">
@@ -781,7 +788,7 @@
       <c r="L3" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -792,7 +799,7 @@
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F4" t="s">
@@ -801,7 +808,7 @@
       <c r="G4" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="K4" t="s">
@@ -810,7 +817,7 @@
       <c r="L4" t="s">
         <v>40</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -821,7 +828,7 @@
       <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F5" t="s">
@@ -830,7 +837,7 @@
       <c r="G5" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="K5" t="s">
@@ -839,7 +846,7 @@
       <c r="L5" t="s">
         <v>65</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="N5" t="s">
@@ -853,7 +860,7 @@
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
@@ -865,7 +872,7 @@
       <c r="G6" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I6" t="s">
@@ -877,7 +884,7 @@
       <c r="L6" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -888,7 +895,7 @@
       <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F7" t="s">
@@ -897,7 +904,7 @@
       <c r="G7" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="K7" t="s">
@@ -906,7 +913,7 @@
       <c r="L7" t="s">
         <v>65</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="M7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -917,7 +924,7 @@
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
@@ -929,7 +936,7 @@
       <c r="G8" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="K8" t="s">
@@ -938,7 +945,7 @@
       <c r="L8" t="s">
         <v>65</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="M8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -949,7 +956,7 @@
       <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F9" t="s">
@@ -958,7 +965,7 @@
       <c r="G9" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I9" t="s">
@@ -970,7 +977,7 @@
       <c r="L9" t="s">
         <v>50</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="M9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -981,54 +988,54 @@
       <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
         <v>23</v>
       </c>
       <c r="K10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L10" t="s">
         <v>50</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="M10" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C11" s="3"/>
+      <c r="C11" s="1"/>
       <c r="K11" t="s">
         <v>63</v>
       </c>
       <c r="L11" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="3" t="s">
+      <c r="M11" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="F12" s="1" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="F12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
       <c r="K12" t="s">
         <v>61</v>
       </c>
       <c r="L12" t="s">
         <v>40</v>
       </c>
-      <c r="M12" s="3" t="s">
+      <c r="M12" s="1" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1039,7 +1046,7 @@
       <c r="B13" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D13" t="s">
@@ -1051,7 +1058,7 @@
       <c r="G13" t="s">
         <v>1</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I13" t="s">
@@ -1063,7 +1070,7 @@
       <c r="L13" t="s">
         <v>40</v>
       </c>
-      <c r="M13" s="3" t="s">
+      <c r="M13" s="1" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1074,86 +1081,83 @@
       <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D14" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I14" s="3" t="s">
+      <c r="G14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="5" t="s">
+      <c r="C15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I15" s="3" t="s">
+      <c r="H15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>43</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="5" t="s">
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I16" s="3"/>
-      <c r="K16" t="s">
-        <v>0</v>
-      </c>
-      <c r="L16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="N16" t="s">
-        <v>3</v>
-      </c>
+      <c r="H16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="K16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1162,29 +1166,32 @@
       <c r="B17" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I17" s="3" t="s">
+      <c r="G17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K17" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>8</v>
+      <c r="K17" t="s">
+        <v>0</v>
+      </c>
+      <c r="L17" t="s">
+        <v>1</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N17" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -1194,69 +1201,69 @@
       <c r="B18" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="5" t="s">
+      <c r="C18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I18" s="3"/>
-      <c r="K18" s="5" t="s">
+      <c r="H18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="K18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C19" s="1"/>
+      <c r="F19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="K19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="K20" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="L18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C19" s="3"/>
-      <c r="F19" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I19" s="3"/>
-      <c r="K19" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="K20" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M20" s="3" t="s">
+      <c r="L20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M20" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1267,27 +1274,36 @@
       <c r="B21" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D21" t="s">
         <v>3</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="K21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D22" t="s">
@@ -1299,56 +1315,44 @@
       <c r="G22" t="s">
         <v>1</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I22" t="s">
         <v>3</v>
       </c>
-      <c r="K22" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>29</v>
       </c>
       <c r="B23" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="4" t="s">
+      <c r="C23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I23" s="3" t="s">
+      <c r="G23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K23" t="s">
-        <v>0</v>
-      </c>
-      <c r="L23" t="s">
-        <v>1</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="N23" t="s">
-        <v>3</v>
-      </c>
+      <c r="K23" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1357,53 +1361,62 @@
       <c r="B24" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="5" t="s">
+      <c r="C24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I24" s="3" t="s">
+      <c r="H24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K24" s="3" t="s">
+      <c r="K24" t="s">
+        <v>0</v>
+      </c>
+      <c r="L24" t="s">
+        <v>1</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" s="1"/>
+      <c r="K25" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F25" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I25" s="3"/>
-      <c r="K25" s="3" t="s">
+    <row r="26" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="K26" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="K26" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
@@ -1413,18 +1426,21 @@
       <c r="B27" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D27" t="s">
         <v>3</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="K27" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -1433,7 +1449,7 @@
       <c r="B28" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D28" t="s">
@@ -1445,7 +1461,7 @@
       <c r="G28" t="s">
         <v>1</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="H28" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I28" t="s">
@@ -1459,22 +1475,22 @@
       <c r="B29" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D29" t="s">
         <v>34</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G29" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I29" s="3" t="s">
+      <c r="G29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1485,22 +1501,22 @@
       <c r="B30" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D30" t="s">
         <v>36</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="G30" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H30" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I30" s="3" t="s">
+      <c r="H30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1511,261 +1527,256 @@
       <c r="B31" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F31" s="5" t="s">
+      <c r="C31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I31" s="3"/>
+      <c r="G31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F32" s="5"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
     </row>
     <row r="33" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F33" s="5"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
     </row>
     <row r="34" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F34" s="5"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
     </row>
     <row r="35" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F35" s="5"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
     </row>
     <row r="36" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F36" s="5"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
     </row>
     <row r="37" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F37" s="5"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
     </row>
     <row r="38" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F38" s="5"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
     </row>
     <row r="39" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F39" s="5"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
     </row>
     <row r="40" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F40" s="5"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
     </row>
     <row r="41" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F41" s="5"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
     </row>
     <row r="42" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F42" s="5"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
     </row>
     <row r="43" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F43" s="5"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
     </row>
     <row r="44" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F44" s="5"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
     </row>
     <row r="45" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
     </row>
     <row r="46" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
     </row>
     <row r="47" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
     </row>
     <row r="48" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
     </row>
     <row r="49" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
     </row>
     <row r="50" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
     </row>
     <row r="51" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
     </row>
     <row r="52" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
     </row>
     <row r="53" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
     </row>
     <row r="54" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
     </row>
     <row r="55" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
     </row>
     <row r="56" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
     </row>
     <row r="57" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
     </row>
     <row r="58" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
-      <c r="I58" s="3"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
     </row>
     <row r="59" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
-      <c r="I59" s="3"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
     </row>
     <row r="60" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-      <c r="H60" s="3"/>
-      <c r="I60" s="3"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
     </row>
     <row r="61" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
-      <c r="I61" s="3"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
     </row>
     <row r="62" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
-      <c r="I62" s="3"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
     </row>
     <row r="63" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-      <c r="H63" s="3"/>
-      <c r="I63" s="3"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
     </row>
     <row r="64" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
-      <c r="H64" s="3"/>
-      <c r="I64" s="3"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
     </row>
     <row r="65" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
-      <c r="H65" s="3"/>
-      <c r="I65" s="3"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
     </row>
     <row r="66" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
-      <c r="H66" s="3"/>
-      <c r="I66" s="3"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
     </row>
     <row r="67" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F67" s="3"/>
-      <c r="G67" s="3"/>
-      <c r="H67" s="3"/>
-      <c r="I67" s="3"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
     </row>
     <row r="68" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
-      <c r="H68" s="3"/>
-      <c r="I68" s="3"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
     </row>
     <row r="69" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F69" s="3"/>
-      <c r="G69" s="3"/>
-      <c r="H69" s="3"/>
-      <c r="I69" s="3"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
     </row>
     <row r="70" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
-      <c r="H70" s="3"/>
-      <c r="I70" s="3"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="K15:N15"/>
-    <mergeCell ref="K22:N22"/>
-    <mergeCell ref="A1:D1"/>
     <mergeCell ref="R1:U1"/>
     <mergeCell ref="A12:D12"/>
     <mergeCell ref="A20:D20"/>
@@ -1773,6 +1784,11 @@
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="F12:I12"/>
     <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="K23:N23"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>